<commit_message>
Added Chase and wells forgo in Account check
Added Chase and wells forgo in Account check
</commit_message>
<xml_diff>
--- a/resources/TestData.xlsx
+++ b/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="AccountCheck" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="254">
   <si>
     <t>RestAddBook</t>
   </si>
@@ -732,6 +732,54 @@
   </si>
   <si>
     <t>Invalid_City_State_Zip_Combination</t>
+  </si>
+  <si>
+    <t>ChaseUsername</t>
+  </si>
+  <si>
+    <t>ChasePassword</t>
+  </si>
+  <si>
+    <t>ac2018demo</t>
+  </si>
+  <si>
+    <t>FormFree2018</t>
+  </si>
+  <si>
+    <t>FormFree2019</t>
+  </si>
+  <si>
+    <t>FormFree2020</t>
+  </si>
+  <si>
+    <t>FormFree2021</t>
+  </si>
+  <si>
+    <t>FormFree2022</t>
+  </si>
+  <si>
+    <t>WellsFargo Username</t>
+  </si>
+  <si>
+    <t>WellsFargo Password</t>
+  </si>
+  <si>
+    <t>ffwellstest19</t>
+  </si>
+  <si>
+    <t>TestWells19a</t>
+  </si>
+  <si>
+    <t>ffwellstest20</t>
+  </si>
+  <si>
+    <t>ffwellstest21</t>
+  </si>
+  <si>
+    <t>ffwellstest22</t>
+  </si>
+  <si>
+    <t>ffwellstest23</t>
   </si>
 </sst>
 </file>
@@ -1101,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W26"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,10 +1171,15 @@
     <col min="17" max="17" width="13.28515625" style="1" customWidth="1"/>
     <col min="18" max="21" width="9.140625" style="1"/>
     <col min="22" max="22" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="23" max="23" width="9.140625" style="1"/>
+    <col min="24" max="24" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.5703125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1196,8 +1249,20 @@
       <c r="W1" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1267,8 +1332,20 @@
       <c r="W2" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
@@ -1338,8 +1415,20 @@
       <c r="W3" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1409,8 +1498,20 @@
       <c r="W4" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1480,8 +1581,20 @@
       <c r="W5" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1551,8 +1664,20 @@
       <c r="W6" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1611,7 +1736,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1670,7 +1795,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1729,7 +1854,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1788,7 +1913,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1847,7 +1972,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1906,7 +2031,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1965,7 +2090,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2024,7 +2149,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -2083,7 +2208,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -6914,7 +7039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>